<commit_message>
adjusted max proficiency level to 10 for topics and subtopics
</commit_message>
<xml_diff>
--- a/Knowledge Base /O level Physics (2023-2025).xlsx
+++ b/Knowledge Base /O level Physics (2023-2025).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muneebshafique/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muneebshafique/Desktop/GSCP/GSCP-II---Adaptive-Learning-Systems/Knowledge Base /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA644735-5061-B94E-91AA-76310155E347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0139F31F-6368-C841-B205-A44F7DDA2AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1180" windowWidth="23860" windowHeight="15180" xr2:uid="{B616A9DC-5DA9-4143-B8C0-05B99904E6D2}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="10000" windowHeight="16880" xr2:uid="{B616A9DC-5DA9-4143-B8C0-05B99904E6D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>Balanced and unbalanced forces</t>
   </si>
   <si>
-    <t>Circular Motion</t>
-  </si>
-  <si>
     <t xml:space="preserve">Momentum </t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t xml:space="preserve">Consequences of thermal energy transfer </t>
   </si>
   <si>
-    <t>Electromagnetic Spectrum</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sound </t>
   </si>
   <si>
@@ -279,22 +273,28 @@
     <t xml:space="preserve">Earth and the Solar System </t>
   </si>
   <si>
-    <t xml:space="preserve">The Earth </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Solar System </t>
-  </si>
-  <si>
     <t xml:space="preserve">Stars and the Universe </t>
   </si>
   <si>
-    <t xml:space="preserve">The Sun as a star </t>
-  </si>
-  <si>
     <t xml:space="preserve">Stars </t>
   </si>
   <si>
-    <t xml:space="preserve">The Universe </t>
+    <t>Circular motion</t>
+  </si>
+  <si>
+    <t>Electromagnetic spectrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The earth </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The solar system </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sun as a star </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The universe </t>
   </si>
 </sst>
 </file>
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C6E09B-2639-A34C-A3F0-8CDD683D48BE}">
   <dimension ref="A1:D191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D164" sqref="D164"/>
+    <sheetView tabSelected="1" topLeftCell="B158" workbookViewId="0">
+      <selection activeCell="B164" sqref="B164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -890,7 +890,7 @@
     <row r="24" spans="2:4">
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>2</v>
@@ -958,7 +958,7 @@
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
@@ -981,10 +981,10 @@
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>2</v>
@@ -1007,7 +1007,7 @@
     <row r="39" spans="2:4">
       <c r="B39" s="2"/>
       <c r="C39" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>2</v>
@@ -1030,7 +1030,7 @@
     <row r="42" spans="2:4">
       <c r="B42" s="2"/>
       <c r="C42" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>2</v>
@@ -1053,7 +1053,7 @@
     <row r="45" spans="2:4">
       <c r="B45" s="2"/>
       <c r="C45" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>2</v>
@@ -1076,7 +1076,7 @@
     <row r="48" spans="2:4">
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>2</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="B51" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="5" t="s">
@@ -1121,13 +1121,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="C54" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>2</v>
@@ -1153,7 +1153,7 @@
       <c r="A57" s="3"/>
       <c r="B57" s="2"/>
       <c r="C57" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>2</v>
@@ -1178,10 +1178,10 @@
     <row r="60" spans="1:4">
       <c r="A60" s="3"/>
       <c r="B60" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C60" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>2</v>
@@ -1207,7 +1207,7 @@
       <c r="A63" s="3"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>2</v>
@@ -1233,7 +1233,7 @@
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>2</v>
@@ -1258,10 +1258,10 @@
     <row r="69" spans="1:4">
       <c r="A69" s="3"/>
       <c r="B69" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C69" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>2</v>
@@ -1287,7 +1287,7 @@
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>2</v>
@@ -1313,7 +1313,7 @@
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>2</v>
@@ -1339,7 +1339,7 @@
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>2</v>
@@ -1363,10 +1363,10 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B81" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="2" t="s">
@@ -1392,10 +1392,10 @@
     <row r="84" spans="1:4">
       <c r="A84" s="3"/>
       <c r="B84" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C84" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>2</v>
@@ -1421,7 +1421,7 @@
       <c r="A87" s="5"/>
       <c r="B87" s="5"/>
       <c r="C87" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>2</v>
@@ -1447,7 +1447,7 @@
       <c r="A90" s="5"/>
       <c r="B90" s="5"/>
       <c r="C90" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>2</v>
@@ -1473,7 +1473,7 @@
       <c r="A93" s="5"/>
       <c r="B93" s="5"/>
       <c r="C93" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D93" s="5" t="s">
         <v>2</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="96" spans="1:4">
       <c r="B96" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>2</v>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="99" spans="1:4">
       <c r="B99" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C99" s="5"/>
       <c r="D99" s="5" t="s">
@@ -1538,10 +1538,10 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C102" s="5"/>
       <c r="D102" s="5" t="s">
@@ -1567,10 +1567,10 @@
     <row r="105" spans="1:4">
       <c r="A105" s="5"/>
       <c r="B105" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>2</v>
@@ -1596,7 +1596,7 @@
       <c r="A108" s="5"/>
       <c r="B108" s="5"/>
       <c r="C108" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>2</v>
@@ -1622,7 +1622,7 @@
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>2</v>
@@ -1648,7 +1648,7 @@
       <c r="A114" s="5"/>
       <c r="B114" s="5"/>
       <c r="C114" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>2</v>
@@ -1672,10 +1672,10 @@
     </row>
     <row r="117" spans="1:4">
       <c r="B117" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C117" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>2</v>
@@ -1693,7 +1693,7 @@
     </row>
     <row r="120" spans="1:4">
       <c r="C120" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>2</v>
@@ -1711,7 +1711,7 @@
     </row>
     <row r="123" spans="1:4">
       <c r="C123" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>2</v>
@@ -1729,10 +1729,10 @@
     </row>
     <row r="126" spans="1:4">
       <c r="B126" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C126" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>2</v>
@@ -1750,7 +1750,7 @@
     </row>
     <row r="129" spans="2:4">
       <c r="C129" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>2</v>
@@ -1768,10 +1768,10 @@
     </row>
     <row r="132" spans="2:4">
       <c r="B132" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>2</v>
@@ -1794,7 +1794,7 @@
     <row r="135" spans="2:4">
       <c r="B135" s="5"/>
       <c r="C135" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>2</v>
@@ -1817,7 +1817,7 @@
     <row r="138" spans="2:4">
       <c r="B138" s="5"/>
       <c r="C138" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>2</v>
@@ -1840,7 +1840,7 @@
     <row r="141" spans="2:4">
       <c r="B141" s="5"/>
       <c r="C141" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>2</v>
@@ -1863,7 +1863,7 @@
     <row r="144" spans="2:4">
       <c r="B144" s="5"/>
       <c r="C144" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>2</v>
@@ -1886,7 +1886,7 @@
     <row r="147" spans="1:4">
       <c r="B147" s="5"/>
       <c r="C147" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>2</v>
@@ -1908,7 +1908,7 @@
     </row>
     <row r="150" spans="1:4">
       <c r="B150" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>2</v>
@@ -1926,13 +1926,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B153" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C153" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="B153" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C153" s="6" t="s">
-        <v>73</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>2</v>
@@ -1958,7 +1958,7 @@
       <c r="A156" s="5"/>
       <c r="B156" s="5"/>
       <c r="C156" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>2</v>
@@ -1983,10 +1983,10 @@
     <row r="159" spans="1:4">
       <c r="A159" s="8"/>
       <c r="B159" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C159" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D159" s="5" t="s">
         <v>2</v>
@@ -2012,7 +2012,7 @@
       <c r="A162" s="5"/>
       <c r="B162" s="5"/>
       <c r="C162" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D162" s="5" t="s">
         <v>2</v>
@@ -2038,7 +2038,7 @@
       <c r="A165" s="5"/>
       <c r="B165" s="5"/>
       <c r="C165" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D165" s="5" t="s">
         <v>2</v>
@@ -2064,7 +2064,7 @@
       <c r="A168" s="5"/>
       <c r="B168" s="5"/>
       <c r="C168" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D168" s="5" t="s">
         <v>2</v>
@@ -2090,7 +2090,7 @@
       <c r="A171" s="5"/>
       <c r="B171" s="5"/>
       <c r="C171" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>2</v>
@@ -2116,7 +2116,7 @@
       <c r="A174" s="5"/>
       <c r="B174" s="5"/>
       <c r="C174" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>2</v>
@@ -2140,13 +2140,13 @@
     </row>
     <row r="177" spans="1:4">
       <c r="A177" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>2</v>
@@ -2172,7 +2172,7 @@
       <c r="A180" s="5"/>
       <c r="B180" s="5"/>
       <c r="C180" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>2</v>
@@ -2197,10 +2197,10 @@
     <row r="183" spans="1:4">
       <c r="A183" s="5"/>
       <c r="B183" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C183" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>2</v>
@@ -2226,7 +2226,7 @@
       <c r="A186" s="5"/>
       <c r="B186" s="5"/>
       <c r="C186" s="6" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>2</v>

</xml_diff>